<commit_message>
Added methods and support for Adding to cart, removing from cart, and viewing cart
</commit_message>
<xml_diff>
--- a/SwagLabs/data_engine/keywords.xlsx
+++ b/SwagLabs/data_engine/keywords.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>Step</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>Step 2</t>
   </si>
   <si>
@@ -203,6 +200,48 @@
   </si>
   <si>
     <t>maximize browser</t>
+  </si>
+  <si>
+    <t>VerifyElementsPresent</t>
+  </si>
+  <si>
+    <t>Verify many objects are present</t>
+  </si>
+  <si>
+    <t>AddToShoppingCart</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>RemoveFromShoppingCart</t>
+  </si>
+  <si>
+    <t>ChangeProductQuantity</t>
+  </si>
+  <si>
+    <t>Step 10</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>Step 11</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Step 12</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>Step 13</t>
   </si>
 </sst>
 </file>
@@ -508,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -614,6 +653,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -639,6 +681,24 @@
     <dxf>
       <alignment horizontal="left" vertical="center"/>
       <border outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="general" vertical="center"/>
+      <border outline="0">
         <left style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </left>
@@ -659,36 +719,13 @@
         <left style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </top>
         <bottom style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center"/>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1144,7 +1181,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1191,7 @@
     <col min="3" max="3" width="24.140625" style="23" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="23" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="40" customWidth="1"/>
     <col min="7" max="7" width="32" style="39" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="24" customWidth="1"/>
     <col min="9" max="11" width="9.140625" style="14" customWidth="1"/>
@@ -1203,73 +1240,65 @@
         <v>11</v>
       </c>
       <c r="G2" s="36"/>
-      <c r="H2" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:13" s="31" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="C3" s="28" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="36"/>
-      <c r="H3" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:13" s="31" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
       <c r="F4" s="32"/>
       <c r="G4" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>12</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="D5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="E5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="F5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="G5" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H5" s="30"/>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
@@ -1278,29 +1307,27 @@
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="C6" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="33" t="s">
+      <c r="E6" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="28" t="s">
+      <c r="G6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H6" s="30"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
@@ -1309,27 +1336,25 @@
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="C7" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="D7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="E7" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="G7" s="36"/>
-      <c r="H7" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H7" s="30"/>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
@@ -1338,22 +1363,22 @@
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>37</v>
-      </c>
       <c r="C8" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="E8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>43</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="30"/>
@@ -1365,20 +1390,20 @@
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>46</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="30"/>
@@ -1390,36 +1415,34 @@
     </row>
     <row r="10" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>48</v>
-      </c>
       <c r="G10" s="36"/>
-      <c r="H10" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H10" s="30"/>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
@@ -1427,9 +1450,7 @@
       <c r="G11" s="36">
         <v>3</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H11" s="30"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
@@ -1438,25 +1459,21 @@
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="25" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="30" t="s">
-        <v>12</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="30"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
@@ -1464,13 +1481,19 @@
       <c r="M12" s="31"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="C13" s="33" t="s">
+        <v>62</v>
+      </c>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="28"/>
-      <c r="G13" s="36"/>
+      <c r="G13" s="36" t="s">
+        <v>70</v>
+      </c>
       <c r="H13" s="30"/>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
@@ -1479,13 +1502,19 @@
       <c r="M13" s="31"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="27" t="s">
+        <v>71</v>
+      </c>
       <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="C14" s="28" t="s">
+        <v>62</v>
+      </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
-      <c r="G14" s="36"/>
+      <c r="G14" s="36" t="s">
+        <v>72</v>
+      </c>
       <c r="H14" s="30"/>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
@@ -1494,11 +1523,18 @@
       <c r="M14" s="31"/>
     </row>
     <row r="15" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="27" t="s">
+        <v>73</v>
+      </c>
       <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
+      <c r="C15" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
+      <c r="G15" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="H15" s="20"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
@@ -1507,7 +1543,7 @@
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="27"/>
       <c r="H16" s="20"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
@@ -1536,58 +1572,45 @@
     </row>
     <row r="19" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
       <c r="H19" s="20"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
       <c r="H20" s="20"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="19"/>
       <c r="H21" s="20"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="19"/>
       <c r="H22" s="20"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="19"/>
       <c r="H23" s="20"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
     </row>
     <row r="24" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="19"/>
       <c r="H24" s="20"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="19"/>
       <c r="H25" s="20"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"id, classname, name, text"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C135:C1048576">
-      <formula1>"OpenBrowser, NavigateTo, InputData, VerifyElementPresent, Click,VerifyTextPresent,VerifyText,MaximizeWindow, MinimizeWindow, RunInBackground"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C134">
-      <formula1>"OpenBrowser, NavigateTo, InputData, VerifyElementPresent, Click,VerifyTextPresent,VerifyText,MaximizeWindow, MinimizeWindow, RunInBackgroun, Delay"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1595,20 +1618,32 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Keyword Maps'!$D$4:$D$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:E12"/>
+  <dimension ref="D2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="37.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
@@ -1616,7 +1651,7 @@
     <row r="2" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
@@ -1632,66 +1667,98 @@
     </row>
     <row r="5" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="9" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>57</v>
+      <c r="D10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="10" t="s">
+      <c r="E17" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to verify sorting using all the criteria.
</commit_message>
<xml_diff>
--- a/SwagLabs/data_engine/keywords.xlsx
+++ b/SwagLabs/data_engine/keywords.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
   <si>
     <t>Step</t>
   </si>
@@ -242,6 +242,45 @@
   </si>
   <si>
     <t>Step 13</t>
+  </si>
+  <si>
+    <t>Step 14</t>
+  </si>
+  <si>
+    <t>Step 15</t>
+  </si>
+  <si>
+    <t>VerifySorting</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Name (A to Z), Name (Z to A), Price (low to high), Price (high to low)</t>
+  </si>
+  <si>
+    <t>Name (Z to A)</t>
+  </si>
+  <si>
+    <t>Step 16</t>
+  </si>
+  <si>
+    <t>Step 17</t>
+  </si>
+  <si>
+    <t>Name (A to Z)</t>
+  </si>
+  <si>
+    <t>Step 18</t>
+  </si>
+  <si>
+    <t>Step 19</t>
+  </si>
+  <si>
+    <t>Price (high to low)</t>
+  </si>
+  <si>
+    <t>Price (low to high)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -587,9 +626,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1181,19 +1217,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="40" customWidth="1"/>
-    <col min="7" max="7" width="32" style="39" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="39" customWidth="1"/>
+    <col min="7" max="7" width="32" style="38" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="23" customWidth="1"/>
     <col min="9" max="11" width="9.140625" style="14" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="14"/>
   </cols>
@@ -1217,325 +1253,325 @@
       <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="31" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:13" s="30" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="1:13" s="31" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" s="30" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="30"/>
-    </row>
-    <row r="4" spans="1:13" s="31" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:13" s="30" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="37" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-    </row>
-    <row r="6" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+    </row>
+    <row r="6" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-    </row>
-    <row r="7" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+    </row>
+    <row r="7" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-    </row>
-    <row r="8" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="G7" s="35"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+    </row>
+    <row r="8" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-    </row>
-    <row r="9" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="G8" s="35"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+    </row>
+    <row r="9" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-    </row>
-    <row r="10" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="G9" s="35"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+    </row>
+    <row r="10" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-    </row>
-    <row r="11" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="G10" s="35"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="36">
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="35">
         <v>3</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-    </row>
-    <row r="12" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+    </row>
+    <row r="12" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="36" t="s">
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-    </row>
-    <row r="13" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+    </row>
+    <row r="13" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="36" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-    </row>
-    <row r="14" spans="1:13" s="34" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+    </row>
+    <row r="14" spans="1:13" s="33" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="36" t="s">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="G15" s="39" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="20"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
@@ -1543,8 +1579,19 @@
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="H16" s="20"/>
+      <c r="A16" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="19"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1552,12 +1599,23 @@
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="H17" s="20"/>
+      <c r="A17" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="19"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
@@ -1565,45 +1623,85 @@
       <c r="M17" s="13"/>
     </row>
     <row r="18" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H18" s="20"/>
+      <c r="A18" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="19"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="19"/>
-      <c r="H19" s="20"/>
+      <c r="A19" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="G19" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="19"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="19"/>
-      <c r="H20" s="20"/>
+      <c r="A20" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="G20" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="19"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="20"/>
+      <c r="A21" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="19"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H22" s="20"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="20"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
     </row>
     <row r="24" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H24" s="20"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H25" s="20"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
     </row>
@@ -1623,7 +1721,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Keyword Maps'!$D$4:$D$17</xm:f>
+            <xm:f>'Keyword Maps'!$D$4:$D$18</xm:f>
           </x14:formula1>
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -1635,131 +1733,157 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:E17"/>
+  <dimension ref="D2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="4" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="11" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="11" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="4:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="10" t="s">
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="F18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>